<commit_message>
Experiment Setting with several updates
</commit_message>
<xml_diff>
--- a/4 Document representation - Sentiment Analysis/Experiment Setting.xlsx
+++ b/4 Document representation - Sentiment Analysis/Experiment Setting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10020"/>
+    <workbookView windowWidth="21600" windowHeight="9915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
   <si>
     <t>No.1</t>
   </si>
@@ -39,6 +39,12 @@
     <t>Stacked Bi-LSTM</t>
   </si>
   <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stacked CNN </t>
+  </si>
+  <si>
     <t>Test Ratio</t>
   </si>
   <si>
@@ -48,6 +54,9 @@
     <t>Accuracy (%)</t>
   </si>
   <si>
+    <t>Testing Ratio 25% ( No.1 )</t>
+  </si>
+  <si>
     <t>Random State</t>
   </si>
   <si>
@@ -60,6 +69,12 @@
     <t>Testing Ratio 40%</t>
   </si>
   <si>
+    <t>Skip-Gram + SVM</t>
+  </si>
+  <si>
+    <t>CBOW + SVM</t>
+  </si>
+  <si>
     <t>Epoch #</t>
   </si>
   <si>
@@ -87,43 +102,112 @@
     <t>No.9</t>
   </si>
   <si>
+    <t>Skip-Gram + LR</t>
+  </si>
+  <si>
+    <t>CBOW + LR</t>
+  </si>
+  <si>
     <t>Sentence Length</t>
   </si>
   <si>
     <t>(+5) 13</t>
   </si>
   <si>
+    <t>Skip-Gram + CNN</t>
+  </si>
+  <si>
+    <t>CBOW + CNN</t>
+  </si>
+  <si>
     <t>Batch Size</t>
   </si>
   <si>
-    <t>CBOW + SVM</t>
+    <t>Skip-Gram + Stacked CNN</t>
+  </si>
+  <si>
+    <t>CBOW + Stacked CNN</t>
   </si>
   <si>
     <t>Lstm Cell</t>
   </si>
   <si>
-    <t>CBOW + LR</t>
+    <t>Skip-Gram + LSTM</t>
+  </si>
+  <si>
+    <t>CBOW + LSTM</t>
   </si>
   <si>
     <t>Layer</t>
   </si>
   <si>
-    <t>CBOW + LSTM</t>
+    <t>Skip-Gram + Bi-LSTM</t>
+  </si>
+  <si>
+    <t>CBOW + Bi-LSTM</t>
   </si>
   <si>
     <t>Comment #</t>
   </si>
   <si>
-    <t>CBOW + Bi-LSTM</t>
+    <t>Skip-Gram + Stacked Bi-LSTM (2 Layers)</t>
+  </si>
+  <si>
+    <t>CBOW + Stacked Bi-LSTM (2 Layers)</t>
   </si>
   <si>
     <t>wordvec dimension #</t>
   </si>
   <si>
-    <t>CBOW + Stacked Bi-LSTM (2 Layers)</t>
-  </si>
-  <si>
     <t>No.2</t>
+  </si>
+  <si>
+    <t>(89.2) 91.7</t>
+  </si>
+  <si>
+    <t>(90.2) 90.8</t>
+  </si>
+  <si>
+    <t>(89.6) 90.4</t>
+  </si>
+  <si>
+    <t>(87.8) 89.1</t>
+  </si>
+  <si>
+    <t>(88.2) 89.1</t>
+  </si>
+  <si>
+    <t>CBOW + Stacked Bi-LSTM (3 Layers)</t>
+  </si>
+  <si>
+    <t>CBOW + Stacked Bi-LSTM (4 Layers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skip-Gram + LSTM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skip-Gram + Bi-LSTM </t>
+  </si>
+  <si>
+    <t>Skip-Gram + Stacked Bi-LSTM (3 Layers)</t>
+  </si>
+  <si>
+    <t>Skip-Gram + Stacked Bi-LSTM (4 Layers)</t>
+  </si>
+  <si>
+    <t>No.1 (CBoW)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>No.10 (Skip-Gram)</t>
+  </si>
+  <si>
+    <t>Skip-Gram+SVM</t>
+  </si>
+  <si>
+    <t>Skip-Gram+LR</t>
   </si>
   <si>
     <t>注：</t>
@@ -179,7 +263,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,10 +291,91 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -229,42 +394,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -273,40 +402,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,15 +418,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -342,22 +447,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,7 +457,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,7 +505,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +529,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,13 +547,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,13 +589,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,19 +625,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,91 +637,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,6 +743,56 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -662,6 +815,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -676,65 +838,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -743,10 +846,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -755,137 +858,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,6 +1016,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -937,12 +1043,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,17 +1064,86 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1033,7 +1214,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1312,26 +1493,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:AA129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.75" style="2" customWidth="1"/>
     <col min="2" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="13.75" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="3" customWidth="1"/>
-    <col min="6" max="8" width="9" style="3"/>
+    <col min="4" max="4" width="15.5833333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.2333333333333" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3"/>
+    <col min="7" max="7" width="12.05" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9" style="3"/>
     <col min="9" max="9" width="12.5" style="3" customWidth="1"/>
-    <col min="10" max="11" width="9" style="3"/>
-    <col min="12" max="12" width="36.25" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="3"/>
+    <col min="10" max="10" width="29.875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="35.625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="39.5" style="3" customWidth="1"/>
+    <col min="14" max="23" width="9" style="3"/>
+    <col min="24" max="24" width="35.625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9" style="3"/>
+    <col min="26" max="26" width="37.125" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:9">
+    <row r="1" s="1" customFormat="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1354,11 +1543,17 @@
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" ht="14.25" spans="1:21">
+      <c r="I1" s="17"/>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:27">
       <c r="A2" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="7">
         <v>0.25</v>
@@ -1382,24 +1577,36 @@
         <v>89.1</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="L2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-    </row>
-    <row r="3" ht="14.25" spans="1:21">
-      <c r="A3" s="6" t="s">
+      <c r="J2" s="18">
+        <v>85.7</v>
+      </c>
+      <c r="K2" s="18">
+        <v>86</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>10</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="X2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="7">
         <v>3</v>
@@ -1411,26 +1618,40 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="X3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" s="31">
+        <v>87.6</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7">
         <v>250</v>
@@ -1442,41 +1663,55 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="21" t="s">
+      <c r="O4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="P4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="Q4" s="24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="9" t="s">
+      <c r="R4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="S4" s="24" t="s">
         <v>24</v>
+      </c>
+      <c r="T4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="25">
+        <v>88.5</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="24">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1485,42 +1720,56 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="L5" s="21" t="s">
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="M5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="21">
+      <c r="N5" s="24">
         <v>50.9</v>
       </c>
-      <c r="N5" s="21">
+      <c r="O5" s="24">
         <v>50.4</v>
       </c>
-      <c r="O5" s="21">
+      <c r="P5" s="24">
         <v>50.8</v>
       </c>
-      <c r="P5" s="21">
+      <c r="Q5" s="24">
         <v>50.5</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="R5" s="24">
         <v>49.4</v>
       </c>
-      <c r="R5" s="21">
+      <c r="S5" s="24">
         <v>48.4</v>
       </c>
-      <c r="S5" s="21">
+      <c r="T5" s="24">
         <v>49.8</v>
       </c>
-      <c r="T5" s="21">
+      <c r="U5" s="24">
         <v>51</v>
       </c>
-      <c r="U5" s="21">
+      <c r="V5" s="24">
         <v>49.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="X5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>88.7</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA5" s="24">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13">
         <v>300</v>
       </c>
       <c r="C6" s="8"/>
@@ -1530,42 +1779,56 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="L6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="21">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="M6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="24">
         <v>84</v>
       </c>
-      <c r="N6" s="21">
+      <c r="O6" s="24">
         <v>85.3</v>
       </c>
-      <c r="O6" s="21">
+      <c r="P6" s="24">
         <v>83.1</v>
       </c>
-      <c r="P6" s="21">
+      <c r="Q6" s="24">
         <v>84.9</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="R6" s="24">
         <v>84.3</v>
       </c>
-      <c r="R6" s="21">
+      <c r="S6" s="24">
         <v>83</v>
       </c>
-      <c r="S6" s="21">
+      <c r="T6" s="24">
         <v>84.3</v>
       </c>
-      <c r="T6" s="21">
+      <c r="U6" s="24">
         <v>83.6</v>
       </c>
-      <c r="U6" s="21">
+      <c r="V6" s="24">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="10">
+      <c r="X6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>88.4</v>
+      </c>
+      <c r="Z6" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="11">
         <v>64</v>
       </c>
       <c r="C7" s="8"/>
@@ -1575,42 +1838,56 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="L7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="21">
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="M7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="24">
         <v>85.5</v>
       </c>
-      <c r="N7" s="21">
+      <c r="O7" s="24">
         <v>86.4</v>
       </c>
-      <c r="O7" s="21">
+      <c r="P7" s="24">
         <v>85.6</v>
       </c>
-      <c r="P7" s="21">
+      <c r="Q7" s="24">
         <v>85.8</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="R7" s="24">
         <v>86</v>
       </c>
-      <c r="R7" s="21">
+      <c r="S7" s="24">
         <v>84.9</v>
       </c>
-      <c r="S7" s="21">
+      <c r="T7" s="24">
         <v>85.8</v>
       </c>
-      <c r="T7" s="21">
+      <c r="U7" s="24">
         <v>84.8</v>
       </c>
-      <c r="U7" s="21">
+      <c r="V7" s="24">
         <v>85.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="X7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>88.9</v>
+      </c>
+      <c r="Z7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA7" s="24">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="11">
         <v>2</v>
       </c>
       <c r="C8" s="8"/>
@@ -1620,42 +1897,56 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="L8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="21">
-        <v>87.6</v>
-      </c>
-      <c r="N8" s="21">
-        <v>87.9</v>
-      </c>
-      <c r="O8" s="21">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="M8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="25">
+        <v>85.7</v>
+      </c>
+      <c r="O8" s="25">
+        <v>86.8</v>
+      </c>
+      <c r="P8" s="25">
+        <v>85.7</v>
+      </c>
+      <c r="Q8" s="25">
+        <v>86.4</v>
+      </c>
+      <c r="R8" s="25">
+        <v>86.3</v>
+      </c>
+      <c r="S8" s="25">
+        <v>85</v>
+      </c>
+      <c r="T8" s="25">
         <v>86.1</v>
       </c>
-      <c r="P8" s="21">
-        <v>88</v>
-      </c>
-      <c r="Q8" s="21">
-        <v>88.6</v>
-      </c>
-      <c r="R8" s="21">
-        <v>86.2</v>
-      </c>
-      <c r="S8" s="21">
-        <v>86.5</v>
-      </c>
-      <c r="T8" s="21">
-        <v>87.3</v>
-      </c>
-      <c r="U8" s="21">
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="12">
+      <c r="U8" s="25">
+        <v>85</v>
+      </c>
+      <c r="V8" s="25">
+        <v>85.9</v>
+      </c>
+      <c r="X8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>89.3</v>
+      </c>
+      <c r="Z8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="13">
         <v>3000</v>
       </c>
       <c r="C9" s="8"/>
@@ -1665,42 +1956,56 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="L9" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="21">
-        <v>88.1</v>
-      </c>
-      <c r="N9" s="21">
-        <v>88.7</v>
-      </c>
-      <c r="O9" s="21">
-        <v>86.4</v>
-      </c>
-      <c r="P9" s="21">
-        <v>89.4</v>
-      </c>
-      <c r="Q9" s="21">
-        <v>89</v>
-      </c>
-      <c r="R9" s="21">
-        <v>87</v>
-      </c>
-      <c r="S9" s="21">
-        <v>88.2</v>
-      </c>
-      <c r="T9" s="21">
-        <v>87.5</v>
-      </c>
-      <c r="U9" s="21">
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="13">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="M9" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="25">
+        <v>86</v>
+      </c>
+      <c r="O9" s="25">
+        <v>87.1</v>
+      </c>
+      <c r="P9" s="25">
+        <v>85.9</v>
+      </c>
+      <c r="Q9" s="25">
+        <v>87.2</v>
+      </c>
+      <c r="R9" s="25">
+        <v>86.8</v>
+      </c>
+      <c r="S9" s="25">
+        <v>85.8</v>
+      </c>
+      <c r="T9" s="25">
+        <v>86</v>
+      </c>
+      <c r="U9" s="25">
+        <v>85.8</v>
+      </c>
+      <c r="V9" s="25">
+        <v>86.1</v>
+      </c>
+      <c r="X9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" s="32">
+        <v>90.3</v>
+      </c>
+      <c r="Z9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA9" s="20">
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="14">
         <v>100</v>
       </c>
       <c r="C10" s="8"/>
@@ -1710,43 +2015,75 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="L10" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="18">
-        <v>89.5</v>
-      </c>
-      <c r="N10" s="18">
-        <v>89.2</v>
-      </c>
-      <c r="O10" s="18">
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="M10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="24">
         <v>87.6</v>
       </c>
-      <c r="P10" s="18">
-        <v>90.2</v>
-      </c>
-      <c r="Q10" s="18">
-        <v>89.6</v>
-      </c>
-      <c r="R10" s="18">
-        <v>87.8</v>
-      </c>
-      <c r="S10" s="18">
-        <v>89.9</v>
-      </c>
-      <c r="T10" s="18">
-        <v>88.9</v>
-      </c>
-      <c r="U10" s="18">
+      <c r="O10" s="24">
+        <v>87.9</v>
+      </c>
+      <c r="P10" s="24">
+        <v>86.1</v>
+      </c>
+      <c r="Q10" s="24">
+        <v>88</v>
+      </c>
+      <c r="R10" s="24">
+        <v>88.6</v>
+      </c>
+      <c r="S10" s="24">
+        <v>86.2</v>
+      </c>
+      <c r="T10" s="24">
+        <v>86.5</v>
+      </c>
+      <c r="U10" s="24">
+        <v>87.3</v>
+      </c>
+      <c r="V10" s="24">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22">
+      <c r="B11" s="15"/>
+      <c r="M11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="24">
+        <v>88.1</v>
+      </c>
+      <c r="O11" s="24">
+        <v>88.7</v>
+      </c>
+      <c r="P11" s="24">
+        <v>86.4</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>89.4</v>
+      </c>
+      <c r="R11" s="24">
+        <v>89</v>
+      </c>
+      <c r="S11" s="24">
+        <v>87</v>
+      </c>
+      <c r="T11" s="24">
         <v>88.2</v>
       </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="14"/>
-    </row>
-    <row r="12" ht="14.25" spans="1:9">
+      <c r="U11" s="24">
+        <v>87.5</v>
+      </c>
+      <c r="V11" s="24">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" spans="1:22">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -1768,10 +2105,46 @@
         <v>6</v>
       </c>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" ht="14.25" spans="1:9">
+      <c r="J12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="20">
+        <v>89.5</v>
+      </c>
+      <c r="O12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" s="20">
+        <v>87.6</v>
+      </c>
+      <c r="Q12" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="R12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="S12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="T12" s="20">
+        <v>89.9</v>
+      </c>
+      <c r="U12" s="20">
+        <v>88.9</v>
+      </c>
+      <c r="V12" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" s="7">
         <v>0.25</v>
@@ -1795,10 +2168,28 @@
         <v>89.2</v>
       </c>
       <c r="I13" s="8"/>
-    </row>
-    <row r="14" ht="14.25" spans="1:9">
+      <c r="J13" s="18">
+        <v>86.8</v>
+      </c>
+      <c r="K13" s="18">
+        <v>87.1</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7">
         <v>20</v>
@@ -1810,10 +2201,24 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-    </row>
-    <row r="15" ht="14.25" spans="1:9">
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="M14" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="7">
         <v>250</v>
@@ -1825,13 +2230,27 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>24</v>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="M15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1840,12 +2259,26 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="M16" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="13">
         <v>300</v>
       </c>
       <c r="C17" s="8"/>
@@ -1855,12 +2288,26 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="10">
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="M17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11">
         <v>64</v>
       </c>
       <c r="C18" s="8"/>
@@ -1870,12 +2317,26 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="10">
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="M18" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="11">
         <v>2</v>
       </c>
       <c r="C19" s="8"/>
@@ -1885,12 +2346,26 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="13">
         <v>3000</v>
       </c>
       <c r="C20" s="8"/>
@@ -1900,12 +2375,26 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="13">
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="M20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="14">
         <v>100</v>
       </c>
       <c r="C21" s="8"/>
@@ -1915,10 +2404,24 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-    </row>
-    <row r="23" ht="14.25" spans="1:9">
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="M21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+    </row>
+    <row r="23" ht="14.25" spans="1:11">
       <c r="A23" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
@@ -1940,10 +2443,16 @@
         <v>6</v>
       </c>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" ht="14.25" spans="1:9">
+      <c r="J23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" spans="1:11">
       <c r="A24" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B24" s="7">
         <v>0.25</v>
@@ -1957,7 +2466,7 @@
       <c r="E24" s="8">
         <v>85.6</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="16">
         <v>86.1</v>
       </c>
       <c r="G24" s="8">
@@ -1967,10 +2476,16 @@
         <v>87.6</v>
       </c>
       <c r="I24" s="8"/>
-    </row>
-    <row r="25" ht="14.25" spans="1:9">
+      <c r="J24" s="18">
+        <v>85.7</v>
+      </c>
+      <c r="K24" s="18">
+        <v>85.9</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" spans="1:11">
       <c r="A25" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" s="7">
         <v>30</v>
@@ -1978,14 +2493,16 @@
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-    </row>
-    <row r="26" ht="14.25" spans="1:9">
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" ht="14.25" spans="1:11">
       <c r="A26" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B26" s="7">
         <v>205</v>
@@ -1993,104 +2510,118 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>24</v>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="12">
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="13">
         <v>300</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="15"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="10">
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="11">
         <v>64</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="15"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="10">
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="11">
         <v>2</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="12">
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="13">
         <v>3000</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="15"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="13">
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="14">
         <v>100</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-    </row>
-    <row r="34" ht="14.25" spans="1:9">
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="34" ht="14.25" spans="1:11">
       <c r="A34" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -2112,10 +2643,16 @@
         <v>6</v>
       </c>
       <c r="I34" s="4"/>
-    </row>
-    <row r="35" ht="14.25" spans="1:9">
+      <c r="J34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" spans="1:11">
       <c r="A35" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" s="7">
         <v>0.3</v>
@@ -2129,7 +2666,7 @@
       <c r="E35" s="8">
         <v>85.78</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="16">
         <v>88</v>
       </c>
       <c r="G35" s="8">
@@ -2139,10 +2676,16 @@
         <v>90.2</v>
       </c>
       <c r="I35" s="8"/>
-    </row>
-    <row r="36" ht="14.25" spans="1:9">
+      <c r="J35" s="18">
+        <v>86.4</v>
+      </c>
+      <c r="K35" s="18">
+        <v>87.2</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" spans="1:11">
       <c r="A36" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B36" s="7">
         <v>20</v>
@@ -2150,14 +2693,16 @@
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="15"/>
+      <c r="F36" s="16"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
-    </row>
-    <row r="37" ht="14.25" spans="1:9">
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" ht="14.25" spans="1:11">
       <c r="A37" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B37" s="7">
         <v>131</v>
@@ -2165,104 +2710,118 @@
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="15"/>
+      <c r="F37" s="16"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>24</v>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
-      <c r="F38" s="15"/>
+      <c r="F38" s="16"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="12">
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="13">
         <v>300</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="15"/>
+      <c r="F39" s="16"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="10">
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="11">
         <v>64</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="15"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="10">
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="11">
         <v>2</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="15"/>
+      <c r="F41" s="16"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="12">
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="13">
         <v>3000</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="15"/>
+      <c r="F42" s="16"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="13">
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="14">
         <v>100</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="15"/>
+      <c r="F43" s="16"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
-    </row>
-    <row r="45" ht="14.25" spans="1:9">
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+    </row>
+    <row r="45" ht="14.25" spans="1:11">
       <c r="A45" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
@@ -2284,10 +2843,16 @@
         <v>6</v>
       </c>
       <c r="I45" s="4"/>
-    </row>
-    <row r="46" ht="14.25" spans="1:9">
+      <c r="J45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" spans="1:11">
       <c r="A46" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B46" s="7">
         <v>0.3</v>
@@ -2301,7 +2866,7 @@
       <c r="E46" s="8">
         <v>86</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="16">
         <v>88.6</v>
       </c>
       <c r="G46" s="8">
@@ -2311,10 +2876,16 @@
         <v>89.5556</v>
       </c>
       <c r="I46" s="8"/>
-    </row>
-    <row r="47" ht="14.25" spans="1:9">
+      <c r="J46" s="18">
+        <v>86.3</v>
+      </c>
+      <c r="K46" s="18">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" spans="1:11">
       <c r="A47" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B47" s="7">
         <v>21</v>
@@ -2322,14 +2893,16 @@
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="15"/>
+      <c r="F47" s="16"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
-    </row>
-    <row r="48" ht="14.25" spans="1:9">
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+    </row>
+    <row r="48" ht="14.25" spans="1:11">
       <c r="A48" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B48" s="7">
         <v>107</v>
@@ -2337,104 +2910,118 @@
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="15"/>
+      <c r="F48" s="16"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>24</v>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="15"/>
+      <c r="F49" s="16"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="12">
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="13">
         <v>300</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="15"/>
+      <c r="F50" s="16"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="10">
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="11">
         <v>64</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
-      <c r="F51" s="15"/>
+      <c r="F51" s="16"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="10">
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="11">
         <v>2</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
-      <c r="F52" s="15"/>
+      <c r="F52" s="16"/>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="12">
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="13">
         <v>3000</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="15"/>
+      <c r="F53" s="16"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" s="13">
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="14">
         <v>100</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="F54" s="15"/>
+      <c r="F54" s="16"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
-    </row>
-    <row r="56" ht="14.25" spans="1:9">
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+    </row>
+    <row r="56" ht="14.25" spans="1:11">
       <c r="A56" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4" t="s">
@@ -2456,10 +3043,16 @@
         <v>6</v>
       </c>
       <c r="I56" s="4"/>
-    </row>
-    <row r="57" ht="14.25" spans="1:9">
+      <c r="J56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" ht="14.25" spans="1:11">
       <c r="A57" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B57" s="7">
         <v>0.3</v>
@@ -2473,7 +3066,7 @@
       <c r="E57" s="8">
         <v>84.89</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="16">
         <v>86.2</v>
       </c>
       <c r="G57" s="8">
@@ -2483,10 +3076,16 @@
         <v>87.8</v>
       </c>
       <c r="I57" s="8"/>
-    </row>
-    <row r="58" ht="14.25" spans="1:9">
+      <c r="J57" s="18">
+        <v>85</v>
+      </c>
+      <c r="K57" s="18">
+        <v>85.8</v>
+      </c>
+    </row>
+    <row r="58" ht="14.25" spans="1:11">
       <c r="A58" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B58" s="7">
         <v>3</v>
@@ -2494,14 +3093,16 @@
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="15"/>
+      <c r="F58" s="16"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
-    </row>
-    <row r="59" ht="14.25" spans="1:9">
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+    </row>
+    <row r="59" ht="14.25" spans="1:11">
       <c r="A59" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B59" s="7">
         <v>149</v>
@@ -2509,104 +3110,118 @@
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
-      <c r="F59" s="15"/>
+      <c r="F59" s="16"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>24</v>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="15"/>
+      <c r="F60" s="16"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="12">
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="13">
         <v>300</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
-      <c r="F61" s="15"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="10">
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="11">
         <v>64</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
-      <c r="F62" s="15"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B63" s="10">
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="11">
         <v>2</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
-      <c r="F63" s="15"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="12">
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="13">
         <v>3000</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
-      <c r="F64" s="15"/>
+      <c r="F64" s="16"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="13">
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="14">
         <v>100</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="15"/>
+      <c r="F65" s="16"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
-    </row>
-    <row r="67" ht="14.25" spans="1:9">
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+    </row>
+    <row r="67" ht="14.25" spans="1:11">
       <c r="A67" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
@@ -2628,10 +3243,16 @@
         <v>6</v>
       </c>
       <c r="I67" s="4"/>
-    </row>
-    <row r="68" ht="14.25" spans="1:9">
+      <c r="J67" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25" spans="1:11">
       <c r="A68" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B68" s="7">
         <v>0.4</v>
@@ -2645,7 +3266,7 @@
       <c r="E68" s="8">
         <v>85.8</v>
       </c>
-      <c r="F68" s="15">
+      <c r="F68" s="16">
         <v>86.5</v>
       </c>
       <c r="G68" s="8">
@@ -2655,10 +3276,16 @@
         <v>89.9</v>
       </c>
       <c r="I68" s="8"/>
-    </row>
-    <row r="69" ht="14.25" spans="1:9">
+      <c r="J68" s="18">
+        <v>86.1</v>
+      </c>
+      <c r="K68" s="18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25" spans="1:11">
       <c r="A69" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B69" s="7">
         <v>20</v>
@@ -2666,14 +3293,16 @@
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
-      <c r="F69" s="15"/>
+      <c r="F69" s="16"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
-    </row>
-    <row r="70" ht="14.25" spans="1:9">
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+    </row>
+    <row r="70" ht="14.25" spans="1:11">
       <c r="A70" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B70" s="7">
         <v>134</v>
@@ -2681,104 +3310,118 @@
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="15"/>
+      <c r="F70" s="16"/>
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>24</v>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="15"/>
+      <c r="F71" s="16"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" s="12">
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="13">
         <v>300</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
-      <c r="F72" s="15"/>
+      <c r="F72" s="16"/>
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B73" s="10">
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="11">
         <v>64</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="15"/>
+      <c r="F73" s="16"/>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B74" s="10">
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" s="11">
         <v>2</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
-      <c r="F74" s="15"/>
+      <c r="F74" s="16"/>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B75" s="12">
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="13">
         <v>3000</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="15"/>
+      <c r="F75" s="16"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B76" s="13">
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" s="14">
         <v>100</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="15"/>
+      <c r="F76" s="16"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
-    </row>
-    <row r="78" ht="14.25" spans="1:9">
+      <c r="J76" s="26"/>
+      <c r="K76" s="26"/>
+    </row>
+    <row r="78" ht="14.25" spans="1:11">
       <c r="A78" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
@@ -2800,10 +3443,16 @@
         <v>6</v>
       </c>
       <c r="I78" s="4"/>
-    </row>
-    <row r="79" ht="14.25" spans="1:9">
+      <c r="J78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25" spans="1:11">
       <c r="A79" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B79" s="7">
         <v>0.4</v>
@@ -2817,7 +3466,7 @@
       <c r="E79" s="8">
         <v>84.8</v>
       </c>
-      <c r="F79" s="15">
+      <c r="F79" s="16">
         <v>87.3</v>
       </c>
       <c r="G79" s="8">
@@ -2827,10 +3476,16 @@
         <v>88.9</v>
       </c>
       <c r="I79" s="8"/>
-    </row>
-    <row r="80" ht="14.25" spans="1:9">
+      <c r="J79" s="18">
+        <v>85</v>
+      </c>
+      <c r="K79" s="18">
+        <v>85.8</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25" spans="1:11">
       <c r="A80" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B80" s="7">
         <v>19</v>
@@ -2838,14 +3493,16 @@
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
-      <c r="F80" s="15"/>
+      <c r="F80" s="16"/>
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
-    </row>
-    <row r="81" ht="14.25" spans="1:9">
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+    </row>
+    <row r="81" ht="14.25" spans="1:11">
       <c r="A81" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B81" s="7">
         <v>117</v>
@@ -2853,104 +3510,118 @@
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
-      <c r="F81" s="15"/>
+      <c r="F81" s="16"/>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>24</v>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
-      <c r="F82" s="15"/>
+      <c r="F82" s="16"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B83" s="12">
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="13">
         <v>300</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
-      <c r="F83" s="15"/>
+      <c r="F83" s="16"/>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84" s="10">
+      <c r="J83" s="21"/>
+      <c r="K83" s="21"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="11">
         <v>64</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
-      <c r="F84" s="15"/>
+      <c r="F84" s="16"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B85" s="10">
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B85" s="11">
         <v>2</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
-      <c r="F85" s="15"/>
+      <c r="F85" s="16"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B86" s="12">
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B86" s="13">
         <v>3000</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
-      <c r="F86" s="15"/>
+      <c r="F86" s="16"/>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B87" s="13">
+      <c r="J86" s="21"/>
+      <c r="K86" s="21"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" s="14">
         <v>100</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
-      <c r="F87" s="15"/>
+      <c r="F87" s="16"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
-    </row>
-    <row r="89" ht="14.25" spans="1:9">
+      <c r="J87" s="26"/>
+      <c r="K87" s="26"/>
+    </row>
+    <row r="89" ht="14.25" spans="1:11">
       <c r="A89" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4" t="s">
@@ -2972,10 +3643,16 @@
         <v>6</v>
       </c>
       <c r="I89" s="4"/>
-    </row>
-    <row r="90" ht="14.25" spans="1:9">
+      <c r="J89" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" ht="14.25" spans="1:11">
       <c r="A90" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B90" s="7">
         <v>0.4</v>
@@ -2989,7 +3666,7 @@
       <c r="E90" s="8">
         <v>85.3</v>
       </c>
-      <c r="F90" s="15">
+      <c r="F90" s="16">
         <v>87.5</v>
       </c>
       <c r="G90" s="8">
@@ -2999,10 +3676,16 @@
         <v>88.2</v>
       </c>
       <c r="I90" s="8"/>
-    </row>
-    <row r="91" ht="14.25" spans="1:9">
+      <c r="J90" s="18">
+        <v>85.9</v>
+      </c>
+      <c r="K90" s="18">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="91" ht="14.25" spans="1:11">
       <c r="A91" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B91" s="7">
         <v>30</v>
@@ -3010,14 +3693,16 @@
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
-      <c r="F91" s="15"/>
+      <c r="F91" s="16"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
-    </row>
-    <row r="92" ht="14.25" spans="1:9">
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+    </row>
+    <row r="92" ht="14.25" spans="1:11">
       <c r="A92" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B92" s="7">
         <v>68</v>
@@ -3025,164 +3710,576 @@
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
-      <c r="F92" s="15"/>
+      <c r="F92" s="16"/>
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>24</v>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
-      <c r="F93" s="15"/>
+      <c r="F93" s="16"/>
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
       <c r="I93" s="8"/>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" s="12">
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" s="13">
         <v>300</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
-      <c r="F94" s="15"/>
+      <c r="F94" s="16"/>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B95" s="10">
+      <c r="J94" s="21"/>
+      <c r="K94" s="21"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" s="11">
         <v>64</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
-      <c r="F95" s="15"/>
+      <c r="F95" s="16"/>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
       <c r="I95" s="8"/>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B96" s="10">
+      <c r="J95" s="21"/>
+      <c r="K95" s="21"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B96" s="11">
         <v>2</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
-      <c r="F96" s="15"/>
+      <c r="F96" s="16"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B97" s="12">
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" s="13">
         <v>3000</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
-      <c r="F97" s="15"/>
+      <c r="F97" s="16"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
       <c r="I97" s="8"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B98" s="13">
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B98" s="14">
         <v>100</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
-      <c r="F98" s="15"/>
+      <c r="F98" s="16"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
-    </row>
-    <row r="104" ht="13.5" spans="1:3">
-      <c r="A104" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C104" s="23"/>
-    </row>
-    <row r="105" ht="17" customHeight="1" spans="1:3">
-      <c r="A105" s="6" t="s">
+      <c r="J98" s="26"/>
+      <c r="K98" s="26"/>
+    </row>
+    <row r="100" ht="14.25" spans="1:11">
+      <c r="A100" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F100" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="G100" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I100" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J100" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="K100" s="51"/>
+    </row>
+    <row r="101" ht="14.25" spans="1:11">
+      <c r="A101" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C101" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D101" s="36">
+        <v>84</v>
+      </c>
+      <c r="E101" s="36">
+        <v>85.5</v>
+      </c>
+      <c r="F101" s="37">
+        <v>85.7</v>
+      </c>
+      <c r="G101" s="37">
+        <v>86</v>
+      </c>
+      <c r="H101" s="36">
+        <v>87.6</v>
+      </c>
+      <c r="I101" s="36">
+        <v>88.1</v>
+      </c>
+      <c r="J101" s="36">
+        <v>89.1</v>
+      </c>
+      <c r="K101" s="36"/>
+    </row>
+    <row r="102" ht="14.25" spans="1:11">
+      <c r="A102" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" s="35">
+        <v>3</v>
+      </c>
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="39"/>
+      <c r="H102" s="36"/>
+      <c r="I102" s="36"/>
+      <c r="J102" s="36"/>
+      <c r="K102" s="36"/>
+    </row>
+    <row r="103" ht="14.25" spans="1:11">
+      <c r="A103" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="35">
+        <v>250</v>
+      </c>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="36"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="39"/>
+      <c r="H103" s="36"/>
+      <c r="I103" s="36"/>
+      <c r="J103" s="36"/>
+      <c r="K103" s="36"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="36"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="36"/>
+      <c r="F104" s="39"/>
+      <c r="G104" s="39"/>
+      <c r="H104" s="36"/>
+      <c r="I104" s="36"/>
+      <c r="J104" s="36"/>
+      <c r="K104" s="36"/>
+    </row>
+    <row r="105" ht="17" customHeight="1" spans="1:11">
+      <c r="A105" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105" s="43">
+        <v>300</v>
+      </c>
+      <c r="C105" s="36"/>
+      <c r="D105" s="36"/>
+      <c r="E105" s="36"/>
+      <c r="F105" s="39"/>
+      <c r="G105" s="39"/>
+      <c r="H105" s="36"/>
+      <c r="I105" s="36"/>
+      <c r="J105" s="36"/>
+      <c r="K105" s="36"/>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C105" s="24"/>
-    </row>
-    <row r="106" ht="14.25" spans="1:3">
-      <c r="A106" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C107" s="15"/>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B108" s="15"/>
-      <c r="C108" s="15"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B109" s="15"/>
-      <c r="C109" s="15"/>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B110" s="15"/>
-      <c r="C110" s="15"/>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="25"/>
+      <c r="B106" s="41">
+        <v>64</v>
+      </c>
+      <c r="C106" s="36"/>
+      <c r="D106" s="36"/>
+      <c r="E106" s="36"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="39"/>
+      <c r="H106" s="36"/>
+      <c r="I106" s="36"/>
+      <c r="J106" s="36"/>
+      <c r="K106" s="36"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B107" s="41">
+        <v>2</v>
+      </c>
+      <c r="C107" s="36"/>
+      <c r="D107" s="36"/>
+      <c r="E107" s="36"/>
+      <c r="F107" s="39"/>
+      <c r="G107" s="39"/>
+      <c r="H107" s="36"/>
+      <c r="I107" s="36"/>
+      <c r="J107" s="36"/>
+      <c r="K107" s="36"/>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B108" s="43">
+        <v>3000</v>
+      </c>
+      <c r="C108" s="36"/>
+      <c r="D108" s="36"/>
+      <c r="E108" s="36"/>
+      <c r="F108" s="39"/>
+      <c r="G108" s="39"/>
+      <c r="H108" s="36"/>
+      <c r="I108" s="36"/>
+      <c r="J108" s="36"/>
+      <c r="K108" s="36"/>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B109" s="44">
+        <v>100</v>
+      </c>
+      <c r="C109" s="36"/>
+      <c r="D109" s="36"/>
+      <c r="E109" s="36"/>
+      <c r="F109" s="45"/>
+      <c r="G109" s="45"/>
+      <c r="H109" s="36"/>
+      <c r="I109" s="36"/>
+      <c r="J109" s="36"/>
+      <c r="K109" s="36"/>
+    </row>
+    <row r="110" ht="14.25" spans="1:11">
+      <c r="A110" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B110" s="33"/>
+      <c r="C110" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E110" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F110" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G110" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H110" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I110" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J110" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="K110" s="51"/>
+    </row>
+    <row r="111" ht="14.25" spans="1:11">
+      <c r="A111" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="C111" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" s="36">
+        <v>87.6</v>
+      </c>
+      <c r="E111" s="36">
+        <v>88.5</v>
+      </c>
+      <c r="F111" s="37">
+        <v>88.7</v>
+      </c>
+      <c r="G111" s="37">
+        <v>88.4</v>
+      </c>
+      <c r="H111" s="46">
+        <v>88.9</v>
+      </c>
+      <c r="I111" s="46">
+        <v>89.3</v>
+      </c>
+      <c r="J111" s="36">
+        <v>90.3</v>
+      </c>
+      <c r="K111" s="36"/>
+    </row>
+    <row r="112" ht="14.25" spans="1:11">
+      <c r="A112" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" s="35">
+        <v>3</v>
+      </c>
+      <c r="C112" s="36"/>
+      <c r="D112" s="36"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="39"/>
+      <c r="G112" s="39"/>
+      <c r="H112" s="46"/>
+      <c r="I112" s="46"/>
+      <c r="J112" s="36"/>
+      <c r="K112" s="36"/>
+    </row>
+    <row r="113" ht="14.25" spans="1:11">
+      <c r="A113" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113" s="35">
+        <v>250</v>
+      </c>
+      <c r="C113" s="36"/>
+      <c r="D113" s="36"/>
+      <c r="E113" s="36"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="39"/>
+      <c r="H113" s="46"/>
+      <c r="I113" s="46"/>
+      <c r="J113" s="36"/>
+      <c r="K113" s="36"/>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="36"/>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
+      <c r="F114" s="39"/>
+      <c r="G114" s="39"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="46"/>
+      <c r="J114" s="36"/>
+      <c r="K114" s="36"/>
+    </row>
+    <row r="115" spans="1:11">
+      <c r="A115" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B115" s="43">
+        <v>300</v>
+      </c>
+      <c r="C115" s="36"/>
+      <c r="D115" s="36"/>
+      <c r="E115" s="36"/>
+      <c r="F115" s="39"/>
+      <c r="G115" s="39"/>
+      <c r="H115" s="46"/>
+      <c r="I115" s="46"/>
+      <c r="J115" s="36"/>
+      <c r="K115" s="36"/>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" s="41">
+        <v>64</v>
+      </c>
+      <c r="C116" s="36"/>
+      <c r="D116" s="36"/>
+      <c r="E116" s="36"/>
+      <c r="F116" s="39"/>
+      <c r="G116" s="39"/>
+      <c r="H116" s="46"/>
+      <c r="I116" s="46"/>
+      <c r="J116" s="36"/>
+      <c r="K116" s="36"/>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B117" s="41">
+        <v>2</v>
+      </c>
+      <c r="C117" s="36"/>
+      <c r="D117" s="36"/>
+      <c r="E117" s="36"/>
+      <c r="F117" s="39"/>
+      <c r="G117" s="39"/>
+      <c r="H117" s="46"/>
+      <c r="I117" s="46"/>
+      <c r="J117" s="36"/>
+      <c r="K117" s="36"/>
+    </row>
+    <row r="118" spans="1:11">
+      <c r="A118" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B118" s="43">
+        <v>3000</v>
+      </c>
+      <c r="C118" s="36"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="39"/>
+      <c r="G118" s="39"/>
+      <c r="H118" s="46"/>
+      <c r="I118" s="46"/>
+      <c r="J118" s="36"/>
+      <c r="K118" s="36"/>
+    </row>
+    <row r="119" spans="1:11">
+      <c r="A119" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B119" s="44">
+        <v>100</v>
+      </c>
+      <c r="C119" s="36"/>
+      <c r="D119" s="36"/>
+      <c r="E119" s="36"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="46"/>
+      <c r="I119" s="46"/>
+      <c r="J119" s="36"/>
+      <c r="K119" s="36"/>
+    </row>
+    <row r="123" ht="13.5" spans="1:3">
+      <c r="A123" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C123" s="48"/>
+    </row>
+    <row r="124" ht="14.25" spans="1:3">
+      <c r="A124" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C124" s="49"/>
+    </row>
+    <row r="125" ht="14.25" spans="1:3">
+      <c r="A125" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125" s="49"/>
+      <c r="C125" s="49"/>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C126" s="16"/>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B128" s="16"/>
+      <c r="C128" s="16"/>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B129" s="16"/>
+      <c r="C129" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="118">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="M2:U2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="N2:V2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="A23:B23"/>
@@ -3199,6 +4296,10 @@
     <mergeCell ref="H78:I78"/>
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="H89:I89"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="J110:K110"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="C13:C21"/>
     <mergeCell ref="C24:C32"/>
@@ -3208,6 +4309,8 @@
     <mergeCell ref="C68:C76"/>
     <mergeCell ref="C79:C87"/>
     <mergeCell ref="C90:C98"/>
+    <mergeCell ref="C101:C109"/>
+    <mergeCell ref="C111:C119"/>
     <mergeCell ref="D2:D10"/>
     <mergeCell ref="D13:D21"/>
     <mergeCell ref="D24:D32"/>
@@ -3217,6 +4320,8 @@
     <mergeCell ref="D68:D76"/>
     <mergeCell ref="D79:D87"/>
     <mergeCell ref="D90:D98"/>
+    <mergeCell ref="D101:D109"/>
+    <mergeCell ref="D111:D119"/>
     <mergeCell ref="E2:E10"/>
     <mergeCell ref="E13:E21"/>
     <mergeCell ref="E24:E32"/>
@@ -3226,6 +4331,8 @@
     <mergeCell ref="E68:E76"/>
     <mergeCell ref="E79:E87"/>
     <mergeCell ref="E90:E98"/>
+    <mergeCell ref="E101:E109"/>
+    <mergeCell ref="E111:E119"/>
     <mergeCell ref="F2:F10"/>
     <mergeCell ref="F13:F21"/>
     <mergeCell ref="F24:F32"/>
@@ -3235,6 +4342,8 @@
     <mergeCell ref="F68:F76"/>
     <mergeCell ref="F79:F87"/>
     <mergeCell ref="F90:F98"/>
+    <mergeCell ref="F101:F109"/>
+    <mergeCell ref="F111:F119"/>
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G13:G21"/>
     <mergeCell ref="G24:G32"/>
@@ -3244,7 +4353,31 @@
     <mergeCell ref="G68:G76"/>
     <mergeCell ref="G79:G87"/>
     <mergeCell ref="G90:G98"/>
-    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="G101:G109"/>
+    <mergeCell ref="G111:G119"/>
+    <mergeCell ref="H101:H109"/>
+    <mergeCell ref="H111:H119"/>
+    <mergeCell ref="I101:I109"/>
+    <mergeCell ref="I111:I119"/>
+    <mergeCell ref="J2:J10"/>
+    <mergeCell ref="J13:J21"/>
+    <mergeCell ref="J24:J32"/>
+    <mergeCell ref="J35:J43"/>
+    <mergeCell ref="J46:J54"/>
+    <mergeCell ref="J57:J65"/>
+    <mergeCell ref="J68:J76"/>
+    <mergeCell ref="J79:J87"/>
+    <mergeCell ref="J90:J98"/>
+    <mergeCell ref="K2:K10"/>
+    <mergeCell ref="K13:K21"/>
+    <mergeCell ref="K24:K32"/>
+    <mergeCell ref="K35:K43"/>
+    <mergeCell ref="K46:K54"/>
+    <mergeCell ref="K57:K65"/>
+    <mergeCell ref="K68:K76"/>
+    <mergeCell ref="K79:K87"/>
+    <mergeCell ref="K90:K98"/>
+    <mergeCell ref="M2:M4"/>
     <mergeCell ref="H2:I10"/>
     <mergeCell ref="H13:I21"/>
     <mergeCell ref="H24:I32"/>
@@ -3254,8 +4387,10 @@
     <mergeCell ref="H68:I76"/>
     <mergeCell ref="H79:I87"/>
     <mergeCell ref="H90:I98"/>
-    <mergeCell ref="B107:C110"/>
-    <mergeCell ref="B105:C106"/>
+    <mergeCell ref="J101:K109"/>
+    <mergeCell ref="B126:C129"/>
+    <mergeCell ref="B124:C125"/>
+    <mergeCell ref="J111:K119"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>